<commit_message>
BPM structure aligned with form
</commit_message>
<xml_diff>
--- a/client/assets/componentsData.xlsx
+++ b/client/assets/componentsData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Office\nocodeai\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Office\nocodeai.cloud\client\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Bpm_Component" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -271,15 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -289,7 +282,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,10 +599,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -612,8 +613,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
@@ -622,10 +623,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -636,10 +637,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="10">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -650,8 +651,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
@@ -660,10 +661,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -674,10 +675,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -688,8 +689,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
@@ -698,8 +699,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
@@ -708,8 +709,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
@@ -718,8 +719,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="3"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="1" t="s">
         <v>34</v>
       </c>
@@ -728,13 +729,13 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="5">
         <v>6</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -742,9 +743,9 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="10" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -752,9 +753,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="10" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -762,8 +763,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
@@ -772,9 +773,9 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="10" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -782,9 +783,9 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -792,13 +793,13 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="A20" s="8">
         <v>7</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -806,9 +807,9 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="10" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -816,13 +817,13 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="8">
         <v>8</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -830,9 +831,9 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="10" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -840,81 +841,115 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="3">
         <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="3">
         <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="3">
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="3">
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="4" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="A9:A13"/>
     <mergeCell ref="B14:B19"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="A9:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>

</xml_diff>